<commit_message>
Find last digit problem slove
</commit_message>
<xml_diff>
--- a/excel/interview problems.xlsx
+++ b/excel/interview problems.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\Pradeeb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="10860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3522,7 +3518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3550,6 +3546,30 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3565,30 +3585,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3872,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3885,103 +3882,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3993,15 +3990,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4098,7 +4095,7 @@
       <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="21" t="s">
         <v>987</v>
       </c>
       <c r="G19" s="4"/>
@@ -4108,7 +4105,7 @@
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="60" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -4861,12 +4858,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="47" t="s">
+      <c r="B66" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="49"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="44"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12484,24 +12481,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="45" t="s">
+      <c r="A540" s="22" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="40"/>
-      <c r="C540" s="40"/>
-      <c r="D540" s="40"/>
-      <c r="E540" s="46"/>
+      <c r="B540" s="23"/>
+      <c r="C540" s="23"/>
+      <c r="D540" s="23"/>
+      <c r="E540" s="24"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="21" t="s">
+      <c r="A541" s="45" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="22"/>
-      <c r="C541" s="22"/>
-      <c r="D541" s="22"/>
-      <c r="E541" s="23"/>
+      <c r="B541" s="46"/>
+      <c r="C541" s="46"/>
+      <c r="D541" s="46"/>
+      <c r="E541" s="47"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12527,12 +12524,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="24" t="s">
+      <c r="B544" s="48" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="25"/>
-      <c r="D544" s="25"/>
-      <c r="E544" s="26"/>
+      <c r="C544" s="49"/>
+      <c r="D544" s="49"/>
+      <c r="E544" s="50"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12540,12 +12537,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="27" t="s">
+      <c r="B545" s="51" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="28"/>
-      <c r="D545" s="28"/>
-      <c r="E545" s="29"/>
+      <c r="C545" s="52"/>
+      <c r="D545" s="52"/>
+      <c r="E545" s="53"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12553,25 +12550,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="30" t="s">
+      <c r="B546" s="54" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="31"/>
-      <c r="D546" s="31"/>
-      <c r="E546" s="32"/>
+      <c r="C546" s="55"/>
+      <c r="D546" s="55"/>
+      <c r="E546" s="56"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="33" t="s">
+      <c r="A547" s="57" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="34"/>
-      <c r="C547" s="34"/>
-      <c r="D547" s="34"/>
-      <c r="E547" s="34"/>
-      <c r="F547" s="34"/>
-      <c r="G547" s="35"/>
+      <c r="B547" s="58"/>
+      <c r="C547" s="58"/>
+      <c r="D547" s="58"/>
+      <c r="E547" s="58"/>
+      <c r="F547" s="58"/>
+      <c r="G547" s="59"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -21224,6 +21221,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -21236,11 +21238,6 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>

</xml_diff>

<commit_message>
division in given number digit wise
</commit_message>
<xml_diff>
--- a/excel/interview problems.xlsx
+++ b/excel/interview problems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="10860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="988">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3547,6 +3547,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3585,7 +3586,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3869,116 +3869,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47" style="3" customWidth="1"/>
+    <col min="2" max="2" width="86.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="30.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3990,15 +3990,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4105,7 +4105,7 @@
       <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -4114,7 +4114,9 @@
       <c r="E20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4131,7 +4133,9 @@
       <c r="E21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4858,12 +4862,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="45"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12481,24 +12485,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="22" t="s">
+      <c r="A540" s="23" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="23"/>
-      <c r="C540" s="23"/>
-      <c r="D540" s="23"/>
-      <c r="E540" s="24"/>
+      <c r="B540" s="24"/>
+      <c r="C540" s="24"/>
+      <c r="D540" s="24"/>
+      <c r="E540" s="25"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="45" t="s">
+      <c r="A541" s="46" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="46"/>
-      <c r="C541" s="46"/>
-      <c r="D541" s="46"/>
-      <c r="E541" s="47"/>
+      <c r="B541" s="47"/>
+      <c r="C541" s="47"/>
+      <c r="D541" s="47"/>
+      <c r="E541" s="48"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12524,12 +12528,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="48" t="s">
+      <c r="B544" s="49" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="49"/>
-      <c r="D544" s="49"/>
-      <c r="E544" s="50"/>
+      <c r="C544" s="50"/>
+      <c r="D544" s="50"/>
+      <c r="E544" s="51"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12537,12 +12541,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="51" t="s">
+      <c r="B545" s="52" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="52"/>
-      <c r="D545" s="52"/>
-      <c r="E545" s="53"/>
+      <c r="C545" s="53"/>
+      <c r="D545" s="53"/>
+      <c r="E545" s="54"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12550,25 +12554,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="54" t="s">
+      <c r="B546" s="55" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="55"/>
-      <c r="D546" s="55"/>
-      <c r="E546" s="56"/>
+      <c r="C546" s="56"/>
+      <c r="D546" s="56"/>
+      <c r="E546" s="57"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="57" t="s">
+      <c r="A547" s="58" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="58"/>
-      <c r="C547" s="58"/>
-      <c r="D547" s="58"/>
-      <c r="E547" s="58"/>
-      <c r="F547" s="58"/>
-      <c r="G547" s="59"/>
+      <c r="B547" s="59"/>
+      <c r="C547" s="59"/>
+      <c r="D547" s="59"/>
+      <c r="E547" s="59"/>
+      <c r="F547" s="59"/>
+      <c r="G547" s="60"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>

</xml_diff>

<commit_message>
GCD( Greatest Common Divisor) OR HCF (Highest Common Factor)
</commit_message>
<xml_diff>
--- a/excel/interview problems.xlsx
+++ b/excel/interview problems.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="989">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3041,6 +3041,9 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Euclidean method</t>
   </si>
 </sst>
 </file>
@@ -3518,7 +3521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3548,21 +3551,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3586,6 +3574,22 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3869,116 +3873,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="86.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="3" customWidth="1"/>
     <col min="4" max="16384" width="30.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="52"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="54"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3990,15 +3994,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4171,7 +4175,9 @@
       <c r="E23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4188,8 +4194,12 @@
       <c r="E24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="21" t="s">
+        <v>987</v>
+      </c>
+      <c r="G24" s="61" t="s">
+        <v>988</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
@@ -4864,12 +4874,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="58" t="s">
+      <c r="B66" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="59"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="60"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="45"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12487,24 +12497,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="38" t="s">
+      <c r="A540" s="23" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="39"/>
-      <c r="C540" s="39"/>
-      <c r="D540" s="39"/>
-      <c r="E540" s="40"/>
+      <c r="B540" s="24"/>
+      <c r="C540" s="24"/>
+      <c r="D540" s="24"/>
+      <c r="E540" s="25"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="23" t="s">
+      <c r="A541" s="46" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="24"/>
-      <c r="C541" s="24"/>
-      <c r="D541" s="24"/>
-      <c r="E541" s="25"/>
+      <c r="B541" s="47"/>
+      <c r="C541" s="47"/>
+      <c r="D541" s="47"/>
+      <c r="E541" s="48"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12530,12 +12540,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="26" t="s">
+      <c r="B544" s="49" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="27"/>
-      <c r="D544" s="27"/>
-      <c r="E544" s="28"/>
+      <c r="C544" s="50"/>
+      <c r="D544" s="50"/>
+      <c r="E544" s="51"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12543,12 +12553,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="29" t="s">
+      <c r="B545" s="52" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="30"/>
-      <c r="D545" s="30"/>
-      <c r="E545" s="31"/>
+      <c r="C545" s="53"/>
+      <c r="D545" s="53"/>
+      <c r="E545" s="54"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12556,25 +12566,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="32" t="s">
+      <c r="B546" s="55" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="33"/>
-      <c r="D546" s="33"/>
-      <c r="E546" s="34"/>
+      <c r="C546" s="56"/>
+      <c r="D546" s="56"/>
+      <c r="E546" s="57"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="35" t="s">
+      <c r="A547" s="58" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="36"/>
-      <c r="C547" s="36"/>
-      <c r="D547" s="36"/>
-      <c r="E547" s="36"/>
-      <c r="F547" s="36"/>
-      <c r="G547" s="37"/>
+      <c r="B547" s="59"/>
+      <c r="C547" s="59"/>
+      <c r="D547" s="59"/>
+      <c r="E547" s="59"/>
+      <c r="F547" s="59"/>
+      <c r="G547" s="60"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -21227,6 +21237,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -21239,11 +21254,6 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>

</xml_diff>

<commit_message>
Print all divisors of a number
</commit_message>
<xml_diff>
--- a/excel/interview problems.xlsx
+++ b/excel/interview problems.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="989">
   <si>
     <t>Curious freaks CODING SHEET by Nandhini</t>
   </si>
@@ -3551,6 +3551,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -3574,22 +3590,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3874,7 +3874,7 @@
   <dimension ref="A1:G1508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3886,103 +3886,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -3994,15 +3994,15 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -4197,7 +4197,7 @@
       <c r="F24" s="21" t="s">
         <v>987</v>
       </c>
-      <c r="G24" s="61" t="s">
+      <c r="G24" s="23" t="s">
         <v>988</v>
       </c>
     </row>
@@ -4215,7 +4215,9 @@
       <c r="E25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="21" t="s">
+        <v>987</v>
+      </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4874,12 +4876,12 @@
       <c r="A66" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="45"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
@@ -12497,24 +12499,24 @@
       <c r="G539" s="12"/>
     </row>
     <row r="540" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A540" s="23" t="s">
+      <c r="A540" s="39" t="s">
         <v>975</v>
       </c>
-      <c r="B540" s="24"/>
-      <c r="C540" s="24"/>
-      <c r="D540" s="24"/>
-      <c r="E540" s="25"/>
+      <c r="B540" s="40"/>
+      <c r="C540" s="40"/>
+      <c r="D540" s="40"/>
+      <c r="E540" s="41"/>
       <c r="F540" s="4"/>
       <c r="G540" s="4"/>
     </row>
     <row r="541" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A541" s="46" t="s">
+      <c r="A541" s="24" t="s">
         <v>986</v>
       </c>
-      <c r="B541" s="47"/>
-      <c r="C541" s="47"/>
-      <c r="D541" s="47"/>
-      <c r="E541" s="48"/>
+      <c r="B541" s="25"/>
+      <c r="C541" s="25"/>
+      <c r="D541" s="25"/>
+      <c r="E541" s="26"/>
       <c r="F541" s="17"/>
       <c r="G541" s="17"/>
     </row>
@@ -12540,12 +12542,12 @@
       <c r="A544" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="B544" s="49" t="s">
+      <c r="B544" s="27" t="s">
         <v>977</v>
       </c>
-      <c r="C544" s="50"/>
-      <c r="D544" s="50"/>
-      <c r="E544" s="51"/>
+      <c r="C544" s="28"/>
+      <c r="D544" s="28"/>
+      <c r="E544" s="29"/>
       <c r="F544" s="17"/>
       <c r="G544" s="17"/>
     </row>
@@ -12553,12 +12555,12 @@
       <c r="A545" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="B545" s="52" t="s">
+      <c r="B545" s="30" t="s">
         <v>979</v>
       </c>
-      <c r="C545" s="53"/>
-      <c r="D545" s="53"/>
-      <c r="E545" s="54"/>
+      <c r="C545" s="31"/>
+      <c r="D545" s="31"/>
+      <c r="E545" s="32"/>
       <c r="F545" s="17"/>
       <c r="G545" s="17"/>
     </row>
@@ -12566,25 +12568,25 @@
       <c r="A546" s="2" t="s">
         <v>980</v>
       </c>
-      <c r="B546" s="55" t="s">
+      <c r="B546" s="33" t="s">
         <v>981</v>
       </c>
-      <c r="C546" s="56"/>
-      <c r="D546" s="56"/>
-      <c r="E546" s="57"/>
+      <c r="C546" s="34"/>
+      <c r="D546" s="34"/>
+      <c r="E546" s="35"/>
       <c r="F546" s="17"/>
       <c r="G546" s="17"/>
     </row>
     <row r="547" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A547" s="58" t="s">
+      <c r="A547" s="36" t="s">
         <v>982</v>
       </c>
-      <c r="B547" s="59"/>
-      <c r="C547" s="59"/>
-      <c r="D547" s="59"/>
-      <c r="E547" s="59"/>
-      <c r="F547" s="59"/>
-      <c r="G547" s="60"/>
+      <c r="B547" s="37"/>
+      <c r="C547" s="37"/>
+      <c r="D547" s="37"/>
+      <c r="E547" s="37"/>
+      <c r="F547" s="37"/>
+      <c r="G547" s="38"/>
     </row>
     <row r="548" spans="1:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="4"/>
@@ -21237,11 +21239,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A541:E541"/>
-    <mergeCell ref="B544:E544"/>
-    <mergeCell ref="B545:E545"/>
-    <mergeCell ref="B546:E546"/>
-    <mergeCell ref="A547:G547"/>
     <mergeCell ref="A540:E540"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:E2"/>
@@ -21254,6 +21251,11 @@
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="B66:E66"/>
+    <mergeCell ref="A541:E541"/>
+    <mergeCell ref="B544:E544"/>
+    <mergeCell ref="B545:E545"/>
+    <mergeCell ref="B546:E546"/>
+    <mergeCell ref="A547:G547"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://www.youtube.com/@curiousfreaks_"/>

</xml_diff>